<commit_message>
feature: 寻址方式 switcher 改为 select
</commit_message>
<xml_diff>
--- a/static/download/bk_nodeman_info_en.xlsx
+++ b/static/download/bk_nodeman_info_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PaaS\git_nodeman\static\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604349E9-32A4-44CD-850C-147B75030CDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F6389-F4A8-480D-B029-E4B809A4F610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3900" yWindow="3255" windowWidth="25350" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="930" windowWidth="28320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetJS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>1.1.1.1</t>
   </si>
@@ -142,7 +142,17 @@
   </si>
   <si>
     <r>
-      <t>Speed ​​limit M/s</t>
+      <t xml:space="preserve">Speed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>​​</t>
     </r>
     <r>
       <rPr>
@@ -153,8 +163,20 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Optional)</t>
+      <t>limit M/s(Optional)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Addressing mode(Optional)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Static</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -162,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +206,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -548,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -569,9 +598,10 @@
     <col min="12" max="12" width="23.625" customWidth="1"/>
     <col min="13" max="13" width="23.375" customWidth="1"/>
     <col min="14" max="14" width="26.5" customWidth="1"/>
+    <col min="15" max="15" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -614,8 +644,11 @@
       <c r="N1" t="s">
         <v>31</v>
       </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -649,8 +682,11 @@
       <c r="M2" t="b">
         <v>1</v>
       </c>
+      <c r="O2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -678,8 +714,11 @@
       <c r="N3">
         <v>3</v>
       </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
feature: 产品页面支持 IPV6 主机导入 (closed #776)
</commit_message>
<xml_diff>
--- a/static/download/bk_nodeman_info_en.xlsx
+++ b/static/download/bk_nodeman_info_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PaaS\git_nodeman\static\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604349E9-32A4-44CD-850C-147B75030CDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F6389-F4A8-480D-B029-E4B809A4F610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3900" yWindow="3255" windowWidth="25350" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="930" windowWidth="28320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetJS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>1.1.1.1</t>
   </si>
@@ -142,7 +142,17 @@
   </si>
   <si>
     <r>
-      <t>Speed ​​limit M/s</t>
+      <t xml:space="preserve">Speed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>​​</t>
     </r>
     <r>
       <rPr>
@@ -153,8 +163,20 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Optional)</t>
+      <t>limit M/s(Optional)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Addressing mode(Optional)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Static</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -162,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +206,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -548,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -569,9 +598,10 @@
     <col min="12" max="12" width="23.625" customWidth="1"/>
     <col min="13" max="13" width="23.375" customWidth="1"/>
     <col min="14" max="14" width="26.5" customWidth="1"/>
+    <col min="15" max="15" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -614,8 +644,11 @@
       <c r="N1" t="s">
         <v>31</v>
       </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -649,8 +682,11 @@
       <c r="M2" t="b">
         <v>1</v>
       </c>
+      <c r="O2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -678,8 +714,11 @@
       <c r="N3">
         <v>3</v>
       </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>